<commit_message>
feat: add options menu for config
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD349CC-76CC-4493-98FA-62B4A1A17763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F694606-71B3-2442-9357-87FAAC04BDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="390" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -430,13 +430,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -462,7 +470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -488,7 +496,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>

</xml_diff>

<commit_message>
feat: add options menu for config (#183)
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD349CC-76CC-4493-98FA-62B4A1A17763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F694606-71B3-2442-9357-87FAAC04BDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="390" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -430,13 +430,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -462,7 +470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -488,7 +496,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>

</xml_diff>

<commit_message>
fix: parsing booleans (#219)
* fix: parsing booleans

* fix: custom columns

* fix: columns
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F694606-71B3-2442-9357-87FAAC04BDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B089E3-B158-8F4B-87FA-8588C45C37A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>time[time]</t>
+  </si>
+  <si>
+    <t>boolean[boolean]</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -85,10 +94,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,9 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -442,9 +456,10 @@
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -469,8 +484,11 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -495,8 +513,11 @@
       <c r="H2" s="2">
         <v>0.625</v>
       </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -520,6 +541,9 @@
       </c>
       <c r="H3" s="2">
         <v>0.66666666666666696</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add missing Edm Type Decimal
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B089E3-B158-8F4B-87FA-8588C45C37A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2C26CA-492D-264A-B99E-97CFF9FB1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>decimal[decimal]</t>
   </si>
 </sst>
 </file>
@@ -94,13 +97,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -440,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +463,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -487,8 +491,11 @@
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -516,8 +523,11 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
+      <c r="J2">
+        <v>15.3</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -544,6 +554,9 @@
       </c>
       <c r="I3" t="s">
         <v>12</v>
+      </c>
+      <c r="J3" s="4">
+        <v>14.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add missing Edm Types (Decimal, Integer) (#221)
* fix: add missing Edm Type Decimal

* fix: add missing integer types
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B089E3-B158-8F4B-87FA-8588C45C37A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2C26CA-492D-264A-B99E-97CFF9FB1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>decimal[decimal]</t>
   </si>
 </sst>
 </file>
@@ -94,13 +97,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -440,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +463,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -487,8 +491,11 @@
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -516,8 +523,11 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
+      <c r="J2">
+        <v>15.3</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -544,6 +554,9 @@
       </c>
       <c r="I3" t="s">
         <v>12</v>
+      </c>
+      <c r="J3" s="4">
+        <v>14.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: special case for Edm.Byte for OData V2 (#519)
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2C26CA-492D-264A-B99E-97CFF9FB1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9DC3A-B534-7746-B9D7-FE9D35DC6349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38740" yWindow="7480" windowWidth="35440" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -62,16 +62,32 @@
   </si>
   <si>
     <t>decimal[decimal]</t>
+  </si>
+  <si>
+    <t>byte[byte]</t>
+  </si>
+  <si>
+    <t>binary[binary]</t>
+  </si>
+  <si>
+    <t>dGhpc2lzYXRlc3Q=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -444,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +479,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -494,8 +510,14 @@
       <c r="J1" t="s">
         <v>13</v>
       </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -526,8 +548,14 @@
       <c r="J2">
         <v>15.3</v>
       </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>254</v>
       </c>
@@ -555,8 +583,14 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <v>14.3</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: parse `Edm.Time` when excel data is text
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9DC3A-B534-7746-B9D7-FE9D35DC6349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FC3F6-0198-0042-8CAE-C4B968E0CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>dGhpc2lzYXRlc3Q=</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -121,6 +124,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -463,7 +467,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,8 +581,8 @@
       <c r="G3" s="1">
         <v>45619</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.66666666666666696</v>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
feat: parse `Edm.Time` when excel data is text (#573)
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9DC3A-B534-7746-B9D7-FE9D35DC6349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FC3F6-0198-0042-8CAE-C4B968E0CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>dGhpc2lzYXRlc3Q=</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -121,6 +124,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -463,7 +467,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,8 +581,8 @@
       <c r="G3" s="1">
         <v>45619</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.66666666666666696</v>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>

</xml_diff>